<commit_message>
Adiciona arquivos com informações do plot do PLSR com filtro SNV
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/plot_infos_plsr_snv.xlsx
+++ b/Partial Least Squares Regression/plot_infos_plsr_snv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>R²</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Offset</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Slope</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Offset</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>R²</t>
         </is>
       </c>
     </row>
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8051743426048511</v>
+        <v>0.8051743426048514</v>
       </c>
       <c r="D2" t="n">
-        <v>2.71163916409923</v>
+        <v>1.148837929164844</v>
       </c>
       <c r="E2" t="n">
-        <v>1.148837929164843</v>
+        <v>2.711639164099223</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8051743426048514</v>
+        <v>0.8051743426048512</v>
       </c>
     </row>
     <row r="3">
@@ -501,40 +501,40 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7793988667851738</v>
+        <v>0.7383382171879158</v>
       </c>
       <c r="D3" t="n">
-        <v>3.067603339747408</v>
+        <v>1.331391679010095</v>
       </c>
       <c r="E3" t="n">
-        <v>1.331391679010094</v>
+        <v>3.067603339747406</v>
       </c>
       <c r="F3" t="n">
-        <v>0.738338217187916</v>
+        <v>0.7793988667851736</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6243669284831971</v>
+        <v>0.7653390937403943</v>
       </c>
       <c r="D4" t="n">
-        <v>1.240089264609238</v>
+        <v>1.088270631842013</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1919195916110745</v>
+        <v>1.31771668119452</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6243669284831987</v>
+        <v>0.9160208818725738</v>
       </c>
     </row>
     <row r="5">
@@ -545,74 +545,74 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Referência</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5180921853576326</v>
+        <v>0.6243669284831987</v>
       </c>
       <c r="D5" t="n">
-        <v>1.592154324702856</v>
+        <v>0.1919195916110745</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2427538713902997</v>
+        <v>1.240089264609229</v>
       </c>
       <c r="F5" t="n">
-        <v>0.399023445923656</v>
+        <v>0.6243669284832003</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Predição</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4946657908947919</v>
+        <v>0.3990234459236567</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5687060065510532</v>
+        <v>0.2427538713902996</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3975020114248576</v>
+        <v>1.592154324702855</v>
       </c>
       <c r="F6" t="n">
-        <v>0.494665790894792</v>
+        <v>0.5180921853576327</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4532763022904974</v>
+        <v>0.4840792817312685</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6175741326214121</v>
+        <v>0.177323052565511</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4348091564766916</v>
+        <v>0.8219452083264076</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3953592680174119</v>
+        <v>0.7495504091221834</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -621,22 +621,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6127065482896521</v>
+        <v>0.494665790894792</v>
       </c>
       <c r="D8" t="n">
-        <v>199.1192575734262</v>
+        <v>0.3975020114248576</v>
       </c>
       <c r="E8" t="n">
-        <v>62.91116033880432</v>
+        <v>0.5687060065510533</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6127065482896514</v>
+        <v>0.494665790894792</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -645,64 +645,184 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4980083127535582</v>
+        <v>0.3953592680174114</v>
       </c>
       <c r="D9" t="n">
-        <v>258.2357080583689</v>
+        <v>0.4348091564766918</v>
       </c>
       <c r="E9" t="n">
-        <v>79.66244398043683</v>
+        <v>0.6175741326214125</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3789994062683447</v>
+        <v>0.4532763022904974</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UBS (%)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6726734889966413</v>
+        <v>0.6378037674957653</v>
       </c>
       <c r="D10" t="n">
-        <v>5.000182059074048</v>
+        <v>0.3090896363122474</v>
       </c>
       <c r="E10" t="n">
-        <v>1.800229857848644</v>
+        <v>-0.2282144515090805</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6726734889966413</v>
+        <v>1.154882760098361</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.6127065482896518</v>
+      </c>
+      <c r="D11" t="n">
+        <v>62.91116033880429</v>
+      </c>
+      <c r="E11" t="n">
+        <v>199.1192575734262</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6127065482896522</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Predição</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.3789994062683451</v>
+      </c>
+      <c r="D12" t="n">
+        <v>79.66244398043682</v>
+      </c>
+      <c r="E12" t="n">
+        <v>258.2357080583688</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4980083127535585</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5474897551728245</v>
+      </c>
+      <c r="D13" t="n">
+        <v>55.06736389728003</v>
+      </c>
+      <c r="E13" t="n">
+        <v>49.75257411922672</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.8799175796427521</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>UBS (%)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.6726734889966415</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.800229857848642</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.000182059074024</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6726734889966427</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Predição</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.6427034599055619</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5.44353426724363</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="C15" t="n">
+        <v>0.597283287976039</v>
+      </c>
+      <c r="D15" t="n">
         <v>1.996812083006219</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.5972832879760388</v>
+      <c r="E15" t="n">
+        <v>5.443534267243627</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.642703459905562</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.7440479612605038</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.213024940458897</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.730532550889199</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.8895905442856631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>